<commit_message>
Update Leave Card 1/18/2024 3:54 pm
</commit_message>
<xml_diff>
--- a/CASUAL/LA CITY MARKET/PRIMO, GRACE.xlsx
+++ b/CASUAL/LA CITY MARKET/PRIMO, GRACE.xlsx
@@ -282,12 +282,6 @@
     <t>UT(0-6-34)</t>
   </si>
   <si>
-    <t>A(4-0-0)</t>
-  </si>
-  <si>
-    <t>6/7,16,18,21/2022</t>
-  </si>
-  <si>
     <t>UT(0-5-28)</t>
   </si>
   <si>
@@ -310,6 +304,12 @@
   </si>
   <si>
     <t>12/21,22,25,26,28/2023</t>
+  </si>
+  <si>
+    <t>6/7,16,18/2022</t>
+  </si>
+  <si>
+    <t>A(3-0-0)</t>
   </si>
 </sst>
 </file>
@@ -694,17 +694,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -714,6 +711,9 @@
     </xf>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1244,7 +1244,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3B5D8F3C-4FD5-4318-83F6-163B56792B3A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B5D8F3C-4FD5-4318-83F6-163B56792B3A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1287,7 +1287,7 @@
         <xdr:cNvPr id="5" name="TextBox 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A0BAE224-67DC-A2F7-0A1F-28CB86DFB7CA}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0BAE224-67DC-A2F7-0A1F-28CB86DFB7CA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1351,7 +1351,7 @@
         <xdr:cNvPr id="4" name="Arrow: Left 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7243AC54-FD55-C7CF-DEF3-E45E6F99CAA1}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7243AC54-FD55-C7CF-DEF3-E45E6F99CAA1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1411,7 +1411,7 @@
         <xdr:cNvPr id="8" name="Oval 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6CEC4AD9-D5D6-0CFD-8D82-CC23F90E3707}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CEC4AD9-D5D6-0CFD-8D82-CC23F90E3707}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1477,7 +1477,7 @@
         <xdr:cNvPr id="9" name="Arrow: Left-Right 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EAE8B24D-B9B9-4AB0-AE94-782594B55A03}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAE8B24D-B9B9-4AB0-AE94-782594B55A03}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1540,7 +1540,7 @@
         <xdr:cNvPr id="10" name="TextBox 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D163C4F0-3D7F-3E52-4B17-0D29F1241915}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D163C4F0-3D7F-3E52-4B17-0D29F1241915}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1638,7 +1638,7 @@
         <xdr:cNvPr id="14" name="Straight Arrow Connector 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{642CA079-93A1-34E3-CEF5-F7D33015D895}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{642CA079-93A1-34E3-CEF5-F7D33015D895}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1697,7 +1697,7 @@
         <xdr:cNvPr id="19" name="TextBox 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{784FECEA-1780-3E7F-7EBB-9F8254797C91}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{784FECEA-1780-3E7F-7EBB-9F8254797C91}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1762,7 +1762,7 @@
         <xdr:cNvPr id="20" name="Picture 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5DCCE859-255F-F039-E92D-1510F02C6167}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DCCE859-255F-F039-E92D-1510F02C6167}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1805,7 +1805,7 @@
         <xdr:cNvPr id="21" name="TextBox 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0A7AA7C6-9540-EB37-E3D2-9A2A68BD6824}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A7AA7C6-9540-EB37-E3D2-9A2A68BD6824}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1880,7 +1880,7 @@
         <xdr:cNvPr id="22" name="TextBox 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F1674299-9801-A253-3871-18715F4FF740}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1674299-9801-A253-3871-18715F4FF740}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2066,7 +2066,7 @@
         <xdr:cNvPr id="23" name="Oval 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{66C92862-99CA-461F-932E-30DFD0874402}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66C92862-99CA-461F-932E-30DFD0874402}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2132,7 +2132,7 @@
         <xdr:cNvPr id="24" name="Straight Arrow Connector 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FD20A152-8288-4C69-BE76-AD8E41A960CE}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD20A152-8288-4C69-BE76-AD8E41A960CE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2190,7 +2190,7 @@
         <xdr:cNvPr id="26" name="Oval 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EE7E56BE-0B3E-4110-A5A9-44C888A46B90}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE7E56BE-0B3E-4110-A5A9-44C888A46B90}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2256,7 +2256,7 @@
         <xdr:cNvPr id="27" name="Straight Arrow Connector 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C33E41C1-1592-4272-A561-4833666913C5}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C33E41C1-1592-4272-A561-4833666913C5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2312,7 +2312,7 @@
         <xdr:cNvPr id="30" name="TextBox 29">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6C655B57-0D66-4740-B73E-75D1E106F99A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C655B57-0D66-4740-B73E-75D1E106F99A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2387,7 +2387,7 @@
         <xdr:cNvPr id="31" name="Picture 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0284C105-1E11-4529-B509-D655B8C5279A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0284C105-1E11-4529-B509-D655B8C5279A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2430,7 +2430,7 @@
         <xdr:cNvPr id="32" name="Oval 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E73E9A40-2B3C-47DC-9C07-7C65795CE0A2}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E73E9A40-2B3C-47DC-9C07-7C65795CE0A2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2496,7 +2496,7 @@
         <xdr:cNvPr id="33" name="Straight Arrow Connector 32">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{32002197-8137-42BA-B3E7-2690738DB64B}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32002197-8137-42BA-B3E7-2690738DB64B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2552,7 +2552,7 @@
         <xdr:cNvPr id="34" name="TextBox 33">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A781E01A-37B6-4259-9759-556FE6893D51}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A781E01A-37B6-4259-9759-556FE6893D51}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3028,9 +3028,9 @@
   <dimension ref="A2:K145"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3990" topLeftCell="A81" activePane="bottomLeft"/>
+      <pane ySplit="3990" topLeftCell="A69" activePane="bottomLeft"/>
       <selection activeCell="G10" sqref="G10"/>
-      <selection pane="bottomLeft" activeCell="F98" sqref="F98"/>
+      <selection pane="bottomLeft" activeCell="J79" sqref="J79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3060,14 +3060,14 @@
         <v>14</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
       <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="25"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="53"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
@@ -3078,16 +3078,16 @@
       <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="55">
+      <c r="F3" s="54">
         <v>41280</v>
       </c>
-      <c r="G3" s="51"/>
+      <c r="G3" s="52"/>
       <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="26"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="57"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="56"/>
     </row>
     <row r="4" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
@@ -3100,16 +3100,16 @@
       <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="51" t="s">
+      <c r="F4" s="52" t="s">
         <v>44</v>
       </c>
-      <c r="G4" s="51"/>
+      <c r="G4" s="52"/>
       <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="26"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="52"/>
+      <c r="J4" s="52"/>
+      <c r="K4" s="53"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
@@ -3135,18 +3135,18 @@
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="53" t="s">
+      <c r="C7" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53" t="s">
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
+      <c r="G7" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="53"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53"/>
+      <c r="H7" s="57"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="57"/>
       <c r="K7" s="14"/>
     </row>
     <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -3193,7 +3193,7 @@
       <c r="D9" s="11"/>
       <c r="E9" s="13">
         <f>SUM(Table13[EARNED])-SUM(Table13[Absence Undertime W/ Pay])</f>
-        <v>36.953000000000003</v>
+        <v>40.453000000000003</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="13" t="str">
@@ -3203,7 +3203,7 @@
       <c r="H9" s="11"/>
       <c r="I9" s="13">
         <f>SUM(Table13[[EARNED ]])-SUM(Table13[Absence Undertime  W/ Pay])</f>
-        <v>80.5</v>
+        <v>83</v>
       </c>
       <c r="J9" s="11"/>
       <c r="K9" s="20"/>
@@ -4343,7 +4343,7 @@
         <v>44652</v>
       </c>
       <c r="B66" s="20" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C66" s="13">
         <v>1.25</v>
@@ -4361,13 +4361,13 @@
       <c r="I66" s="9"/>
       <c r="J66" s="11"/>
       <c r="K66" s="20" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="40"/>
       <c r="B67" s="20" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C67" s="13"/>
       <c r="D67" s="39">
@@ -4389,7 +4389,7 @@
         <v>44682</v>
       </c>
       <c r="B68" s="20" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C68" s="13">
         <v>1.25</v>
@@ -4413,13 +4413,13 @@
         <v>44713</v>
       </c>
       <c r="B69" s="20" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="C69" s="13">
         <v>1.25</v>
       </c>
       <c r="D69" s="39">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E69" s="9"/>
       <c r="F69" s="20"/>
@@ -4431,13 +4431,13 @@
       <c r="I69" s="9"/>
       <c r="J69" s="11"/>
       <c r="K69" s="20" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="40"/>
       <c r="B70" s="20" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C70" s="13"/>
       <c r="D70" s="39">
@@ -5021,13 +5021,15 @@
       <c r="B96" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="C96" s="13"/>
+      <c r="C96" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D96" s="39"/>
       <c r="E96" s="9"/>
       <c r="F96" s="20"/>
-      <c r="G96" s="13" t="str">
-        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G96" s="13">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H96" s="39"/>
       <c r="I96" s="9"/>
@@ -5055,7 +5057,7 @@
       <c r="I97" s="9"/>
       <c r="J97" s="11"/>
       <c r="K97" s="49" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.25">
@@ -5065,13 +5067,15 @@
       <c r="B98" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="C98" s="13"/>
+      <c r="C98" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D98" s="39"/>
       <c r="E98" s="9"/>
       <c r="F98" s="20"/>
-      <c r="G98" s="13" t="str">
-        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G98" s="13">
+        <f>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H98" s="39"/>
       <c r="I98" s="9"/>
@@ -5860,17 +5864,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G7:J7"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="J3:K3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G7:J7"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4">
@@ -5938,14 +5942,14 @@
         <v>14</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
       <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="25"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="53"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
@@ -5956,14 +5960,14 @@
       <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="55"/>
-      <c r="G3" s="51"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="52"/>
       <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="26"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="57"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="56"/>
     </row>
     <row r="4" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
@@ -5976,16 +5980,16 @@
       <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="51" t="s">
+      <c r="F4" s="52" t="s">
         <v>44</v>
       </c>
-      <c r="G4" s="51"/>
+      <c r="G4" s="52"/>
       <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="26"/>
-      <c r="J4" s="51"/>
-      <c r="K4" s="52"/>
+      <c r="J4" s="52"/>
+      <c r="K4" s="53"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
@@ -6011,18 +6015,18 @@
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="53" t="s">
+      <c r="C7" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53" t="s">
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
+      <c r="G7" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="53"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53"/>
+      <c r="H7" s="57"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="57"/>
       <c r="K7" s="14"/>
     </row>
     <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -6273,7 +6277,7 @@
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="40"/>
       <c r="B18" s="20" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C18" s="13"/>
       <c r="D18" s="39">
@@ -6289,7 +6293,7 @@
       <c r="I18" s="9"/>
       <c r="J18" s="11"/>
       <c r="K18" s="20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>